<commit_message>
Added new json and excel files
</commit_message>
<xml_diff>
--- a/structured_attribute_output_00170112.xlsx
+++ b/structured_attribute_output_00170112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaydutonde/Desktop/Barry_Callibaut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BAC67A-B853-7E4D-8A20-A5CC8DC04D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF68029-9C66-2447-82F5-1B19ADCA7F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>